<commit_message>
created Model.ipynb and modified other files
</commit_message>
<xml_diff>
--- a/data/stats.xlsx
+++ b/data/stats.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="911" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="928" uniqueCount="92">
   <si>
     <t>Coversion Rate</t>
   </si>
@@ -102,43 +102,58 @@
     <t>Coeficient</t>
   </si>
   <si>
+    <t>Opportunity Amount &lt; 1500000</t>
+  </si>
+  <si>
     <t>Deal Size Category_7</t>
+  </si>
+  <si>
+    <t>Opportunity Amount &lt; 800000</t>
   </si>
   <si>
     <t>Deal Size Category_6</t>
   </si>
   <si>
+    <t>Opportunity Amount &gt; 700000</t>
+  </si>
+  <si>
+    <t>Opportunity Amount &lt; 700000</t>
+  </si>
+  <si>
+    <t>Opportunity Amount &lt; 500000</t>
+  </si>
+  <si>
+    <t>POS_Telecoverage</t>
+  </si>
+  <si>
+    <t>Opportunity Amount &gt; 800000</t>
+  </si>
+  <si>
+    <t>Opportunity Amount &gt; 600000</t>
+  </si>
+  <si>
     <t>Deal Size Category_5</t>
+  </si>
+  <si>
+    <t>Category_Tires &amp; Wheels</t>
+  </si>
+  <si>
+    <t>Region_Northwest</t>
+  </si>
+  <si>
+    <t>Deal Size Category_2</t>
   </si>
   <si>
     <t>Deal Size Category_4</t>
   </si>
   <si>
-    <t>Deal Size Category_3</t>
-  </si>
-  <si>
-    <t>Deal Size Category_2</t>
-  </si>
-  <si>
-    <t>POS_Telecoverage</t>
-  </si>
-  <si>
-    <t>Category_Tires &amp; Wheels</t>
-  </si>
-  <si>
-    <t>Opportunity Amount &gt; 600000</t>
-  </si>
-  <si>
-    <t>Opportunity Amount &gt; 700000</t>
-  </si>
-  <si>
     <t>Competitor_Unknown</t>
   </si>
   <si>
-    <t>Region_Northwest</t>
+    <t>Client Size By Revenue_5</t>
   </si>
   <si>
-    <t>Client Size By Revenue_5</t>
+    <t>Client Size By Employee Count_2</t>
   </si>
   <si>
     <t>POS_Other</t>
@@ -147,16 +162,10 @@
     <t>Client Size By Employee Count_5</t>
   </si>
   <si>
-    <t>Client Size By Employee Count_2</t>
-  </si>
-  <si>
-    <t>Opportunity Amount &gt; 800000</t>
+    <t>Opportunity Amount &gt; 1000000</t>
   </si>
   <si>
     <t>Region_Southwest</t>
-  </si>
-  <si>
-    <t>Client Size By Revenue_2</t>
   </si>
   <si>
     <t>POS_Telesales</t>
@@ -165,37 +174,34 @@
     <t>Category_Performance &amp; Non-auto</t>
   </si>
   <si>
+    <t>Client Size By Employee Count_4</t>
+  </si>
+  <si>
+    <t>Client Size By Revenue_2</t>
+  </si>
+  <si>
     <t>Region_Southeast</t>
   </si>
   <si>
-    <t>Client Size By Employee Count_4</t>
-  </si>
-  <si>
-    <t>Opportunity Amount &gt; 300000</t>
+    <t>Client Size By Employee Count_3</t>
   </si>
   <si>
     <t>Client Size By Revenue_3</t>
   </si>
   <si>
-    <t>Client Size By Employee Count_3</t>
+    <t>Region_Pacific</t>
   </si>
   <si>
     <t>Region_Northeast</t>
   </si>
   <si>
-    <t>Region_Pacific</t>
+    <t>Deal Size Category_3</t>
   </si>
   <si>
     <t>Client Size By Revenue_4</t>
   </si>
   <si>
     <t>Region_Midwest</t>
-  </si>
-  <si>
-    <t>Opportunity Amount &gt; 5000</t>
-  </si>
-  <si>
-    <t>Opportunity Amount &gt; 150000</t>
   </si>
   <si>
     <t>POS_Reseller</t>
@@ -207,43 +213,88 @@
     <t>Category_Car Electronics</t>
   </si>
   <si>
+    <t>Opportunity Amount &lt; 600000</t>
+  </si>
+  <si>
+    <t>Opportunity Amount &lt; 250000</t>
+  </si>
+  <si>
     <t>Opportunity Amount &gt; 1000</t>
+  </si>
+  <si>
+    <t>Opportunity Amount &gt; 10000</t>
+  </si>
+  <si>
+    <t>Opportunity Amount &gt; 25000</t>
+  </si>
+  <si>
+    <t>Opportunity Amount &gt; 100000</t>
+  </si>
+  <si>
+    <t>Opportunity Amount &gt; 5000</t>
+  </si>
+  <si>
+    <t>Opportunity Amount &lt; 100000</t>
+  </si>
+  <si>
+    <t>Opportunity Amount &lt; 25000</t>
+  </si>
+  <si>
+    <t>Opportunity Amount &lt; 150000</t>
+  </si>
+  <si>
+    <t>Opportunity Amount &lt; 5000</t>
+  </si>
+  <si>
+    <t>Opportunity Amount &lt; 50000</t>
+  </si>
+  <si>
+    <t>Opportunity Amount &lt; 400000</t>
+  </si>
+  <si>
+    <t>Opportunity Amount &lt; 10000</t>
+  </si>
+  <si>
+    <t>Opportunity Amount &gt; 50000</t>
+  </si>
+  <si>
+    <t>Opportunity Amount &lt; 1000000</t>
+  </si>
+  <si>
+    <t>Revenue From Client Past Two Years_4</t>
+  </si>
+  <si>
+    <t>Opportunity Amount &lt; 200000</t>
   </si>
   <si>
     <t>Opportunity Amount &gt; 400000</t>
   </si>
   <si>
-    <t>Opportunity Amount &gt; 25000</t>
+    <t>Opportunity Amount &gt; 300000</t>
+  </si>
+  <si>
+    <t>Opportunity Amount &gt; 150000</t>
   </si>
   <si>
     <t>Opportunity Amount &gt; 200000</t>
   </si>
   <si>
-    <t>Opportunity Amount &gt; 10000</t>
+    <t>Revenue From Client Past Two Years_3</t>
   </si>
   <si>
-    <t>Opportunity Amount &gt; 100000</t>
+    <t>Opportunity Amount &gt; 500000</t>
+  </si>
+  <si>
+    <t>Revenue From Client Past Two Years_2</t>
   </si>
   <si>
     <t>Opportunity Amount &gt; 250000</t>
   </si>
   <si>
-    <t>Opportunity Amount &gt; 50000</t>
+    <t>Revenue From Client Past Two Years_1</t>
   </si>
   <si>
-    <t>Revenue From Client Past Two Years_4</t>
-  </si>
-  <si>
-    <t>Opportunity Amount &gt; 500000</t>
-  </si>
-  <si>
-    <t>Revenue From Client Past Two Years_3</t>
-  </si>
-  <si>
-    <t>Revenue From Client Past Two Years_2</t>
-  </si>
-  <si>
-    <t>Revenue From Client Past Two Years_1</t>
+    <t>Opportunity Amount &lt; 300000</t>
   </si>
 </sst>
 </file>
@@ -18712,7 +18763,7 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B49"/>
+  <dimension ref="A1:B66"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -18728,7 +18779,7 @@
         <v>27</v>
       </c>
       <c r="B2">
-        <v>-10.39495294954587</v>
+        <v>-6.939633873331229</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -18736,7 +18787,7 @@
         <v>28</v>
       </c>
       <c r="B3">
-        <v>-8.247080983628823</v>
+        <v>-5.527185074322019</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -18744,7 +18795,7 @@
         <v>29</v>
       </c>
       <c r="B4">
-        <v>-6.338135198558676</v>
+        <v>-2.236279411676732</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -18752,7 +18803,7 @@
         <v>30</v>
       </c>
       <c r="B5">
-        <v>-4.470612102385786</v>
+        <v>-2.060590304364239</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -18760,7 +18811,7 @@
         <v>31</v>
       </c>
       <c r="B6">
-        <v>-2.75033072517234</v>
+        <v>-1.777044912875483</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -18768,7 +18819,7 @@
         <v>32</v>
       </c>
       <c r="B7">
-        <v>-1.707057759321309</v>
+        <v>-1.681807208628339</v>
       </c>
     </row>
     <row r="8" spans="1:2">
@@ -18776,7 +18827,7 @@
         <v>33</v>
       </c>
       <c r="B8">
-        <v>-1.332512049059616</v>
+        <v>-1.412448799009194</v>
       </c>
     </row>
     <row r="9" spans="1:2">
@@ -18784,7 +18835,7 @@
         <v>34</v>
       </c>
       <c r="B9">
-        <v>-0.2584030774161273</v>
+        <v>-1.260737449773282</v>
       </c>
     </row>
     <row r="10" spans="1:2">
@@ -18792,7 +18843,7 @@
         <v>35</v>
       </c>
       <c r="B10">
-        <v>-0.152139533136461</v>
+        <v>-0.9795805875390046</v>
       </c>
     </row>
     <row r="11" spans="1:2">
@@ -18800,7 +18851,7 @@
         <v>36</v>
       </c>
       <c r="B11">
-        <v>-0.1294291723664877</v>
+        <v>-0.7712545717361659</v>
       </c>
     </row>
     <row r="12" spans="1:2">
@@ -18808,7 +18859,7 @@
         <v>37</v>
       </c>
       <c r="B12">
-        <v>-0.1183638323059282</v>
+        <v>-0.6878411981693952</v>
       </c>
     </row>
     <row r="13" spans="1:2">
@@ -18816,7 +18867,7 @@
         <v>38</v>
       </c>
       <c r="B13">
-        <v>-0.1101991002226014</v>
+        <v>-0.2581571898719109</v>
       </c>
     </row>
     <row r="14" spans="1:2">
@@ -18824,7 +18875,7 @@
         <v>39</v>
       </c>
       <c r="B14">
-        <v>-0.09428523458085854</v>
+        <v>-0.1621776615663869</v>
       </c>
     </row>
     <row r="15" spans="1:2">
@@ -18832,7 +18883,7 @@
         <v>40</v>
       </c>
       <c r="B15">
-        <v>-0.05856319799870321</v>
+        <v>-0.1560359730969999</v>
       </c>
     </row>
     <row r="16" spans="1:2">
@@ -18840,7 +18891,7 @@
         <v>41</v>
       </c>
       <c r="B16">
-        <v>-0.05818226603659372</v>
+        <v>-0.1500991996522717</v>
       </c>
     </row>
     <row r="17" spans="1:2">
@@ -18848,7 +18899,7 @@
         <v>42</v>
       </c>
       <c r="B17">
-        <v>-0.04912315499004433</v>
+        <v>-0.1391273140944808</v>
       </c>
     </row>
     <row r="18" spans="1:2">
@@ -18856,7 +18907,7 @@
         <v>43</v>
       </c>
       <c r="B18">
-        <v>-0.04237489747398801</v>
+        <v>-0.1011055924866702</v>
       </c>
     </row>
     <row r="19" spans="1:2">
@@ -18864,7 +18915,7 @@
         <v>44</v>
       </c>
       <c r="B19">
-        <v>-0.02946158089495177</v>
+        <v>-0.05541413434382469</v>
       </c>
     </row>
     <row r="20" spans="1:2">
@@ -18872,7 +18923,7 @@
         <v>45</v>
       </c>
       <c r="B20">
-        <v>-0.02309367302645306</v>
+        <v>-0.05537793870631925</v>
       </c>
     </row>
     <row r="21" spans="1:2">
@@ -18880,7 +18931,7 @@
         <v>46</v>
       </c>
       <c r="B21">
-        <v>0.004959916760251366</v>
+        <v>-0.02743676828376685</v>
       </c>
     </row>
     <row r="22" spans="1:2">
@@ -18888,7 +18939,7 @@
         <v>47</v>
       </c>
       <c r="B22">
-        <v>0.01424002861256498</v>
+        <v>0</v>
       </c>
     </row>
     <row r="23" spans="1:2">
@@ -18896,7 +18947,7 @@
         <v>48</v>
       </c>
       <c r="B23">
-        <v>0.02249354491935444</v>
+        <v>0.004393777114749361</v>
       </c>
     </row>
     <row r="24" spans="1:2">
@@ -18904,7 +18955,7 @@
         <v>49</v>
       </c>
       <c r="B24">
-        <v>0.02553389602586186</v>
+        <v>0.008055282051123522</v>
       </c>
     </row>
     <row r="25" spans="1:2">
@@ -18912,7 +18963,7 @@
         <v>50</v>
       </c>
       <c r="B25">
-        <v>0.03562299195153539</v>
+        <v>0.008196743063353001</v>
       </c>
     </row>
     <row r="26" spans="1:2">
@@ -18920,7 +18971,7 @@
         <v>51</v>
       </c>
       <c r="B26">
-        <v>0.03739488734013503</v>
+        <v>0.009548385559475542</v>
       </c>
     </row>
     <row r="27" spans="1:2">
@@ -18928,7 +18979,7 @@
         <v>52</v>
       </c>
       <c r="B27">
-        <v>0.04104825453120586</v>
+        <v>0.01614071704645391</v>
       </c>
     </row>
     <row r="28" spans="1:2">
@@ -18936,7 +18987,7 @@
         <v>53</v>
       </c>
       <c r="B28">
-        <v>0.05703303371879558</v>
+        <v>0.01791690768178388</v>
       </c>
     </row>
     <row r="29" spans="1:2">
@@ -18944,7 +18995,7 @@
         <v>54</v>
       </c>
       <c r="B29">
-        <v>0.09021496463827665</v>
+        <v>0.01950298737272416</v>
       </c>
     </row>
     <row r="30" spans="1:2">
@@ -18952,7 +19003,7 @@
         <v>55</v>
       </c>
       <c r="B30">
-        <v>0.1030051141119457</v>
+        <v>0.02522245168138035</v>
       </c>
     </row>
     <row r="31" spans="1:2">
@@ -18960,7 +19011,7 @@
         <v>56</v>
       </c>
       <c r="B31">
-        <v>0.1599626138943598</v>
+        <v>0.02647066573052741</v>
       </c>
     </row>
     <row r="32" spans="1:2">
@@ -18968,7 +19019,7 @@
         <v>57</v>
       </c>
       <c r="B32">
-        <v>0.1822606403195873</v>
+        <v>0.05847413352479494</v>
       </c>
     </row>
     <row r="33" spans="1:2">
@@ -18976,7 +19027,7 @@
         <v>58</v>
       </c>
       <c r="B33">
-        <v>0.1989871491271807</v>
+        <v>0.1033349428439141</v>
       </c>
     </row>
     <row r="34" spans="1:2">
@@ -18984,7 +19035,7 @@
         <v>59</v>
       </c>
       <c r="B34">
-        <v>0.3544381943996283</v>
+        <v>0.1149792450890467</v>
       </c>
     </row>
     <row r="35" spans="1:2">
@@ -18992,7 +19043,7 @@
         <v>60</v>
       </c>
       <c r="B35">
-        <v>0.3930070216702036</v>
+        <v>0.1222506332726698</v>
       </c>
     </row>
     <row r="36" spans="1:2">
@@ -19000,7 +19051,7 @@
         <v>61</v>
       </c>
       <c r="B36">
-        <v>0.4569062410002899</v>
+        <v>0.3256259525853997</v>
       </c>
     </row>
     <row r="37" spans="1:2">
@@ -19008,7 +19059,7 @@
         <v>62</v>
       </c>
       <c r="B37">
-        <v>0.5058683955911599</v>
+        <v>0.3493955740015249</v>
       </c>
     </row>
     <row r="38" spans="1:2">
@@ -19016,7 +19067,7 @@
         <v>63</v>
       </c>
       <c r="B38">
-        <v>0.6725646970666691</v>
+        <v>0.3830181436576884</v>
       </c>
     </row>
     <row r="39" spans="1:2">
@@ -19024,7 +19075,7 @@
         <v>64</v>
       </c>
       <c r="B39">
-        <v>0.8334730987138427</v>
+        <v>0.61212581016317</v>
       </c>
     </row>
     <row r="40" spans="1:2">
@@ -19032,7 +19083,7 @@
         <v>65</v>
       </c>
       <c r="B40">
-        <v>0.9473095741894804</v>
+        <v>0.648141505355007</v>
       </c>
     </row>
     <row r="41" spans="1:2">
@@ -19040,7 +19091,7 @@
         <v>66</v>
       </c>
       <c r="B41">
-        <v>0.9514437024049903</v>
+        <v>0.851826258322658</v>
       </c>
     </row>
     <row r="42" spans="1:2">
@@ -19048,7 +19099,7 @@
         <v>67</v>
       </c>
       <c r="B42">
-        <v>1.030315968404335</v>
+        <v>0.9285736608932371</v>
       </c>
     </row>
     <row r="43" spans="1:2">
@@ -19056,7 +19107,7 @@
         <v>68</v>
       </c>
       <c r="B43">
-        <v>1.16640333997766</v>
+        <v>0.9417053407178654</v>
       </c>
     </row>
     <row r="44" spans="1:2">
@@ -19064,7 +19115,7 @@
         <v>69</v>
       </c>
       <c r="B44">
-        <v>1.569042739278886</v>
+        <v>1.295855238212496</v>
       </c>
     </row>
     <row r="45" spans="1:2">
@@ -19072,7 +19123,7 @@
         <v>70</v>
       </c>
       <c r="B45">
-        <v>1.751889212903288</v>
+        <v>1.305965798225456</v>
       </c>
     </row>
     <row r="46" spans="1:2">
@@ -19080,7 +19131,7 @@
         <v>71</v>
       </c>
       <c r="B46">
-        <v>2.208462891733369</v>
+        <v>1.335982703524365</v>
       </c>
     </row>
     <row r="47" spans="1:2">
@@ -19088,7 +19139,7 @@
         <v>72</v>
       </c>
       <c r="B47">
-        <v>2.324010018252452</v>
+        <v>1.382746960332757</v>
       </c>
     </row>
     <row r="48" spans="1:2">
@@ -19096,7 +19147,7 @@
         <v>73</v>
       </c>
       <c r="B48">
-        <v>2.723745314478602</v>
+        <v>1.393470421993614</v>
       </c>
     </row>
     <row r="49" spans="1:2">
@@ -19104,7 +19155,143 @@
         <v>74</v>
       </c>
       <c r="B49">
-        <v>2.916756702502155</v>
+        <v>1.46245103607736</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2">
+      <c r="A50" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="B50">
+        <v>1.48608190317662</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2">
+      <c r="A51" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="B51">
+        <v>1.502331698125935</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2">
+      <c r="A52" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="B52">
+        <v>1.538782933429707</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2">
+      <c r="A53" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="B53">
+        <v>1.561398754893629</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2">
+      <c r="A54" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="B54">
+        <v>1.583482590393009</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2">
+      <c r="A55" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="B55">
+        <v>1.843494631730819</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2">
+      <c r="A56" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="B56">
+        <v>1.910307626268267</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2">
+      <c r="A57" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="B57">
+        <v>1.932790626035331</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2">
+      <c r="A58" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="B58">
+        <v>1.96642652539062</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2">
+      <c r="A59" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="B59">
+        <v>2.032158917394971</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2">
+      <c r="A60" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B60">
+        <v>2.181795253150293</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2">
+      <c r="A61" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="B61">
+        <v>2.33156511099337</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2">
+      <c r="A62" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="B62">
+        <v>2.530815313236761</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2">
+      <c r="A63" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="B63">
+        <v>2.674484168553326</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2">
+      <c r="A64" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="B64">
+        <v>2.675726861948516</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2">
+      <c r="A65" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="B65">
+        <v>2.926876266517279</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2">
+      <c r="A66" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="B66">
+        <v>3.095470235370601</v>
       </c>
     </row>
   </sheetData>

</xml_diff>